<commit_message>
working on social network of NTU group to determine if one group, and daily activity pattern
</commit_message>
<xml_diff>
--- a/grid_additionalinfo.xlsx
+++ b/grid_additionalinfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zoe Goldsborough\Documents\GitHub\camtrap_coiba\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{919CC0F1-7A47-4DAC-85A8-E90BB15F8AA9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7626504-9C2F-4237-B328-287DFD1DFBAF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8484" xr2:uid="{0C9E6875-CDDB-4DDE-ABCB-A6D11B52ABED}"/>
   </bookViews>
@@ -592,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B304FBA-40FF-4CC7-BCD4-D4951BEE2B9F}">
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="G54" sqref="G54"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>